<commit_message>
table + head + position  add db
</commit_message>
<xml_diff>
--- a/upload_files/1test.xlsx
+++ b/upload_files/1test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MacBookKO/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82266FC1-DA23-5D48-8A4B-EA98B788401A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C444D09-36A8-4F4A-889B-8118FB4F7695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1840" windowWidth="28040" windowHeight="17360" xr2:uid="{95CEA91B-7431-A44E-A30F-92C2E6028308}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>manager</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>ка</t>
+  </si>
+  <si>
+    <t>юрист</t>
+  </si>
+  <si>
+    <t>садовник</t>
   </si>
 </sst>
 </file>
@@ -508,7 +514,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +586,7 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -626,7 +632,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>

</xml_diff>